<commit_message>
Balance Tranfer and Report Gen
</commit_message>
<xml_diff>
--- a/src/test/resources/Exceldata/LoanElibilityData.xlsx
+++ b/src/test/resources/Exceldata/LoanElibilityData.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanilped\Documents\Java Training\MagicBricks\src\test\resources\Exceldata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Basic Java\MagicBricksAutomation\src\test\resources\Exceldata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5A32CAD-9008-44FB-A1A6-268B6D0F505B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C010C92-B9F2-4B4A-88C2-9C3BBC7DA6BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2800" yWindow="2800" windowWidth="14400" windowHeight="8170" activeTab="1" xr2:uid="{CD5858B3-2AB2-4248-86D4-F801C4828A70}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{CD5858B3-2AB2-4248-86D4-F801C4828A70}"/>
   </bookViews>
   <sheets>
-    <sheet name="LoanEligibiltyData" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
+    <sheet name="LoanEligibiltyDataPositive" sheetId="1" r:id="rId1"/>
+    <sheet name="LoanEligibiltyDataNegative" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="11">
   <si>
     <t>Monthly_Income</t>
   </si>
@@ -45,6 +45,21 @@
   </si>
   <si>
     <t>Monthly_EMI</t>
+  </si>
+  <si>
+    <t>1522.08 Cr</t>
+  </si>
+  <si>
+    <t>6.99 Cr</t>
+  </si>
+  <si>
+    <t>1.67 Lac</t>
+  </si>
+  <si>
+    <t>1.68 Lac</t>
+  </si>
+  <si>
+    <t>167.99 Cr</t>
   </si>
 </sst>
 </file>
@@ -95,9 +110,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,100 +457,200 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD81A895-4557-4157-BB02-505B4DD6CAA3}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F4"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="1">
-        <v>100000</v>
-      </c>
-      <c r="B2" s="1">
-        <v>20000</v>
-      </c>
-      <c r="C2" s="1">
-        <v>8.5</v>
-      </c>
-      <c r="D2" s="1">
-        <v>20</v>
-      </c>
-      <c r="E2" s="1">
-        <v>5609000</v>
-      </c>
-      <c r="F2" s="1">
-        <v>56000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="1">
-        <v>50000</v>
-      </c>
-      <c r="B3" s="1">
-        <v>0</v>
-      </c>
-      <c r="C3" s="1">
-        <v>7.5</v>
-      </c>
-      <c r="D3" s="1">
-        <v>15</v>
-      </c>
-      <c r="E3" s="1">
-        <v>2800000</v>
-      </c>
-      <c r="F3" s="1">
-        <v>27000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="1">
-        <v>150000</v>
-      </c>
-      <c r="B4" s="1">
-        <v>50000</v>
-      </c>
-      <c r="C4" s="1">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>10000</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3">
+        <v>5</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>10001</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3">
+        <v>5</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="4">
+        <v>99999999</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0</v>
+      </c>
+      <c r="D4" s="3">
+        <v>5</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="4">
+        <v>100000000</v>
+      </c>
+      <c r="B5" s="5">
+        <v>0</v>
+      </c>
+      <c r="C5" s="5">
+        <v>0</v>
+      </c>
+      <c r="D5" s="3">
+        <v>5</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>10000</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0</v>
+      </c>
+      <c r="C6" s="3">
+        <v>50</v>
+      </c>
+      <c r="D6" s="3">
+        <v>30</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="4">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>10001</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0</v>
+      </c>
+      <c r="C7" s="3">
+        <v>50</v>
+      </c>
+      <c r="D7" s="3">
+        <v>30</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="1">
-        <v>25</v>
-      </c>
-      <c r="E4" s="1">
-        <v>7500000</v>
-      </c>
-      <c r="F4" s="1">
-        <v>72000</v>
+      <c r="F7" s="4">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="4">
+        <v>99999999</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0</v>
+      </c>
+      <c r="C8" s="3">
+        <v>50</v>
+      </c>
+      <c r="D8" s="3">
+        <v>30</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="4">
+        <v>100000000</v>
+      </c>
+      <c r="B9" s="5">
+        <v>0</v>
+      </c>
+      <c r="C9" s="3">
+        <v>50</v>
+      </c>
+      <c r="D9" s="3">
+        <v>30</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -535,15 +660,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22AA7065-2AC7-46BE-B563-5402E60A3AA5}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F4"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -563,64 +691,60 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="1">
-        <v>100000</v>
-      </c>
-      <c r="B2" s="1">
-        <v>20000</v>
-      </c>
-      <c r="C2" s="1">
-        <v>8.5</v>
-      </c>
-      <c r="D2" s="1">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>9999</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>-1</v>
+      </c>
+      <c r="D2">
         <v>20</v>
       </c>
-      <c r="E2" s="1">
-        <v>5609000</v>
-      </c>
-      <c r="F2" s="1">
-        <v>56000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="1">
-        <v>50000</v>
-      </c>
-      <c r="B3" s="1">
-        <v>0</v>
-      </c>
-      <c r="C3" s="1">
-        <v>7.5</v>
-      </c>
-      <c r="D3" s="1">
-        <v>15</v>
-      </c>
-      <c r="E3" s="1">
-        <v>2800000</v>
-      </c>
-      <c r="F3" s="1">
-        <v>27000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="1">
-        <v>150000</v>
-      </c>
-      <c r="B4" s="1">
-        <v>50000</v>
-      </c>
-      <c r="C4" s="1">
-        <v>9</v>
-      </c>
-      <c r="D4" s="1">
-        <v>25</v>
-      </c>
-      <c r="E4" s="1">
-        <v>7500000</v>
-      </c>
-      <c r="F4" s="1">
-        <v>72000</v>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>100000001</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>-1</v>
+      </c>
+      <c r="D3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>9999</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>51</v>
+      </c>
+      <c r="D4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>100000001</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>51</v>
+      </c>
+      <c r="D5">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -636,9 +760,9 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1">
         <v>80000</v>
       </c>
@@ -658,7 +782,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>120000</v>
       </c>
@@ -678,7 +802,7 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>40000</v>
       </c>
@@ -698,7 +822,7 @@
         <v>22000</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>200000</v>
       </c>
@@ -718,7 +842,7 @@
         <v>110000</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>60000</v>
       </c>
@@ -738,7 +862,7 @@
         <v>25000</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>90000</v>
       </c>
@@ -758,7 +882,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>100000</v>
       </c>

</xml_diff>